<commit_message>
R Sachen und Lit
</commit_message>
<xml_diff>
--- a/Projekt 3/P3_Lisa.xlsx
+++ b/Projekt 3/P3_Lisa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lisah\Documents\GitHub\fallstudien\Projekt 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7760266A-22CE-4799-9111-5D8D13A9AF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9872EB73-1347-4933-BA9D-C20539BFCE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="846" activeTab="2" xr2:uid="{BA959CBC-5258-4760-9119-2EC40842E906}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="846" firstSheet="2" activeTab="2" xr2:uid="{BA959CBC-5258-4760-9119-2EC40842E906}"/>
   </bookViews>
   <sheets>
     <sheet name="Abschlusstestverfahren Welch" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="76">
   <si>
     <t>Elementarhypothesen</t>
   </si>
@@ -274,7 +274,7 @@
 glaube ich, weiß nicht so ganz was eig getestet wird</t>
   </si>
   <si>
-    <t>auch anova!</t>
+    <t>2.65e-07</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -475,6 +475,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1373,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD52753A-8070-42B4-AE35-03CE98649BFC}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D30" sqref="D29:D30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1628,7 +1631,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="C15" s="17"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="9" t="s">
         <v>54</v>
       </c>
@@ -1641,11 +1644,9 @@
     </row>
     <row r="16" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="7"/>
-      <c r="C16" t="s">
+      <c r="C16" s="17"/>
+      <c r="D16" s="20" t="s">
         <v>75</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>25</v>
@@ -1658,9 +1659,10 @@
   <mergeCells count="3">
     <mergeCell ref="G3:G8"/>
     <mergeCell ref="D9:D11"/>
-    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="C12:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1668,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85DB0F0-EF4A-4E89-B1F6-054EE7D2143A}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>